<commit_message>
exp 1 graphs added
</commit_message>
<xml_diff>
--- a/Experiment 1/Trace Files/DroppedGraph.xlsx
+++ b/Experiment 1/Trace Files/DroppedGraph.xlsx
@@ -256,19 +256,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>43</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>57</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>56</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -362,19 +362,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>26</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>57</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -468,19 +468,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>5</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>74</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>120</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -571,22 +571,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>169</c:v>
+                  <c:v>167</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>241</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -602,11 +602,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1406073936"/>
-        <c:axId val="1406074480"/>
+        <c:axId val="1025540768"/>
+        <c:axId val="1025542400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1406073936"/>
+        <c:axId val="1025540768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -705,7 +705,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1406074480"/>
+        <c:crossAx val="1025542400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -713,7 +713,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1406074480"/>
+        <c:axId val="1025542400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="250"/>
@@ -822,7 +822,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1406073936"/>
+        <c:crossAx val="1025540768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1760,7 +1760,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.3"/>
@@ -1864,7 +1864,7 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1872,16 +1872,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1889,16 +1889,16 @@
         <v>7</v>
       </c>
       <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
         <v>5</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>5</v>
-      </c>
-      <c r="E8">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1906,16 +1906,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C9">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D9">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="E9">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1923,16 +1923,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C10">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D10">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="E10">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1940,16 +1940,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="C11">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="D11">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="E11">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>